<commit_message>
Add module specific logging to TimeSync and Event Records.  Publish Event Records to MQTT topic.  Modified Event FIFO to use activeTail and readCommit() to delay commitment of FIFO read until records have been successfully published.
</commit_message>
<xml_diff>
--- a/docs/ApplianceData.xlsx
+++ b/docs/ApplianceData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicholas.Weber.DRINKWORKS\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ian.whitehead\GitHub\drinkworks-freertos\modules\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DE5D89A-22A4-4F86-A37F-951763F4A081}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30680539-A5F5-4CD4-94E9-10D1D40A602B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B99E4D13-F1A0-47FA-9245-944F8FF25CEA}"/>
+    <workbookView xWindow="23374" yWindow="-2931" windowWidth="23015" windowHeight="12360" activeTab="1" xr2:uid="{B99E4D13-F1A0-47FA-9245-944F8FF25CEA}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Overview" sheetId="3" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="110">
   <si>
     <t>Shadow Data</t>
   </si>
@@ -339,9 +339,6 @@
     <t>Dispense Shadow</t>
   </si>
   <si>
-    <t>Event Record Topic:</t>
-  </si>
-  <si>
     <t>On connection to AWS or on new record creation</t>
   </si>
   <si>
@@ -352,6 +349,24 @@
   </si>
   <si>
     <t>MZ Firmware String</t>
+  </si>
+  <si>
+    <t>LastPublishedIndex</t>
+  </si>
+  <si>
+    <t>Index of Last Published Event Record</t>
+  </si>
+  <si>
+    <t>Homebar-event-record-devel</t>
+  </si>
+  <si>
+    <t>Event Record Topic, devel:</t>
+  </si>
+  <si>
+    <t>Event Record Topic, prod:</t>
+  </si>
+  <si>
+    <t>Homebar-event-record-prod</t>
   </si>
 </sst>
 </file>
@@ -389,7 +404,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -443,20 +458,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -485,6 +491,15 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -500,16 +515,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2712,33 +2719,35 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{184FE990-6DFE-49C0-8AF5-25BB7F59DB88}">
   <dimension ref="C3:J29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C15" sqref="C15:D15"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="40.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="31.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.42578125" customWidth="1"/>
+    <col min="3" max="3" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="40.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="31.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.44140625" customWidth="1"/>
     <col min="10" max="10" width="28" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C3" s="14" t="s">
+    <row r="3" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C3" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="14"/>
-      <c r="F3" s="14" t="s">
+      <c r="D3" s="19"/>
+      <c r="F3" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="G3" s="14"/>
-      <c r="I3" s="14" t="s">
+      <c r="G3" s="19"/>
+      <c r="I3" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="J3" s="14"/>
-    </row>
-    <row r="4" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="J3" s="19"/>
+    </row>
+    <row r="4" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C4" s="2" t="s">
         <v>4</v>
       </c>
@@ -2758,7 +2767,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C5" s="5" t="s">
         <v>1</v>
       </c>
@@ -2778,7 +2787,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="6" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C6" s="5" t="s">
         <v>2</v>
       </c>
@@ -2798,7 +2807,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="7" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C7" s="5" t="s">
         <v>23</v>
       </c>
@@ -2818,7 +2827,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="8" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C8" s="5" t="s">
         <v>24</v>
       </c>
@@ -2838,7 +2847,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="9" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C9" s="5" t="s">
         <v>16</v>
       </c>
@@ -2858,7 +2867,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="10" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C10" s="6" t="s">
         <v>17</v>
       </c>
@@ -2878,7 +2887,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="11" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C11" s="6" t="s">
         <v>19</v>
       </c>
@@ -2898,7 +2907,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="12" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C12" s="6" t="s">
         <v>20</v>
       </c>
@@ -2918,7 +2927,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="13" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C13" s="6" t="s">
         <v>21</v>
       </c>
@@ -2938,7 +2947,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="14" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C14" s="6" t="s">
         <v>18</v>
       </c>
@@ -2958,9 +2967,13 @@
         <v>83</v>
       </c>
     </row>
-    <row r="15" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C15" s="23"/>
-      <c r="D15" s="23"/>
+    <row r="15" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C15" s="24" t="s">
+        <v>104</v>
+      </c>
+      <c r="D15" s="24" t="s">
+        <v>105</v>
+      </c>
       <c r="F15" s="3" t="s">
         <v>49</v>
       </c>
@@ -2968,7 +2981,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="16" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C16" s="13"/>
       <c r="D16" s="13"/>
       <c r="F16" s="3" t="s">
@@ -2979,7 +2992,7 @@
       </c>
       <c r="I16" s="8"/>
     </row>
-    <row r="17" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C17" s="13"/>
       <c r="D17" s="13"/>
       <c r="F17" s="3" t="s">
@@ -2990,9 +3003,9 @@
       </c>
       <c r="I17" s="8"/>
     </row>
-    <row r="18" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C18" s="24"/>
-      <c r="D18" s="24"/>
+    <row r="18" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C18" s="18"/>
+      <c r="D18" s="18"/>
       <c r="F18" s="3" t="s">
         <v>52</v>
       </c>
@@ -3001,9 +3014,9 @@
       </c>
       <c r="I18" s="8"/>
     </row>
-    <row r="19" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C19" s="24"/>
-      <c r="D19" s="24"/>
+    <row r="19" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C19" s="18"/>
+      <c r="D19" s="18"/>
       <c r="F19" s="3" t="s">
         <v>53</v>
       </c>
@@ -3011,9 +3024,9 @@
         <v>71</v>
       </c>
     </row>
-    <row r="20" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C20" s="24"/>
-      <c r="D20" s="24"/>
+    <row r="20" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C20" s="18"/>
+      <c r="D20" s="18"/>
       <c r="F20" s="3" t="s">
         <v>54</v>
       </c>
@@ -3021,7 +3034,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="21" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:9" x14ac:dyDescent="0.3">
       <c r="F21" s="3" t="s">
         <v>55</v>
       </c>
@@ -3029,42 +3042,42 @@
         <v>73</v>
       </c>
     </row>
-    <row r="24" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C24" s="13"/>
       <c r="D24" s="13"/>
       <c r="E24" s="13"/>
       <c r="F24" s="13"/>
       <c r="G24" s="13"/>
     </row>
-    <row r="25" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C25" s="15"/>
-      <c r="D25" s="15"/>
-      <c r="E25" s="15"/>
-      <c r="F25" s="15"/>
-      <c r="G25" s="15"/>
-    </row>
-    <row r="26" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C25" s="20"/>
+      <c r="D25" s="20"/>
+      <c r="E25" s="20"/>
+      <c r="F25" s="20"/>
+      <c r="G25" s="20"/>
+    </row>
+    <row r="26" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C26" s="13"/>
       <c r="D26" s="13"/>
       <c r="E26" s="13"/>
       <c r="F26" s="13"/>
       <c r="G26" s="13"/>
     </row>
-    <row r="27" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C27" s="13"/>
       <c r="D27" s="13"/>
       <c r="E27" s="13"/>
       <c r="F27" s="13"/>
       <c r="G27" s="13"/>
     </row>
-    <row r="28" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C28" s="13"/>
       <c r="D28" s="13"/>
       <c r="E28" s="13"/>
       <c r="F28" s="13"/>
       <c r="G28" s="13"/>
     </row>
-    <row r="29" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C29" s="13"/>
       <c r="D29" s="13"/>
       <c r="E29" s="13"/>
@@ -3079,36 +3092,37 @@
     <mergeCell ref="C25:G25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC8F59E4-AA7B-4E98-A353-BDF065CC0E98}">
-  <dimension ref="C2:H17"/>
+  <dimension ref="C2:H18"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="40.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.140625" customWidth="1"/>
-    <col min="6" max="6" width="18.7109375" customWidth="1"/>
-    <col min="7" max="7" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="40.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.109375" customWidth="1"/>
+    <col min="6" max="6" width="18.6640625" customWidth="1"/>
+    <col min="7" max="7" width="16.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C2" s="14" t="s">
+    <row r="2" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C2" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-    </row>
-    <row r="3" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+    </row>
+    <row r="3" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C3" s="2" t="s">
         <v>4</v>
       </c>
@@ -3126,7 +3140,7 @@
       </c>
       <c r="H3" s="7"/>
     </row>
-    <row r="4" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C4" s="5" t="s">
         <v>1</v>
       </c>
@@ -3143,7 +3157,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C5" s="5" t="s">
         <v>2</v>
       </c>
@@ -3160,7 +3174,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C6" s="5" t="s">
         <v>23</v>
       </c>
@@ -3177,7 +3191,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C7" s="5" t="s">
         <v>24</v>
       </c>
@@ -3194,7 +3208,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C8" s="5" t="s">
         <v>16</v>
       </c>
@@ -3211,12 +3225,12 @@
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C9" s="22" t="s">
+    <row r="9" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C9" s="17" t="s">
+        <v>102</v>
+      </c>
+      <c r="D9" s="4" t="s">
         <v>103</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>104</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>84</v>
@@ -3228,7 +3242,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C10" s="6" t="s">
         <v>17</v>
       </c>
@@ -3245,7 +3259,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C11" s="6" t="s">
         <v>19</v>
       </c>
@@ -3262,7 +3276,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C12" s="6" t="s">
         <v>20</v>
       </c>
@@ -3279,7 +3293,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C13" s="6" t="s">
         <v>21</v>
       </c>
@@ -3296,7 +3310,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C14" s="6" t="s">
         <v>18</v>
       </c>
@@ -3313,53 +3327,70 @@
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C15" s="16" t="s">
+    <row r="15" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C15" s="24" t="s">
+        <v>104</v>
+      </c>
+      <c r="D15" s="24" t="s">
+        <v>105</v>
+      </c>
+      <c r="E15" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="F15" s="25" t="s">
+        <v>86</v>
+      </c>
+      <c r="G15" s="25" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C16" s="21" t="s">
         <v>92</v>
       </c>
-      <c r="D15" s="16"/>
-      <c r="E15" s="16"/>
-      <c r="F15" s="16"/>
-      <c r="G15" s="16"/>
-    </row>
-    <row r="16" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C16" s="3" t="s">
+      <c r="D16" s="21"/>
+      <c r="E16" s="21"/>
+      <c r="F16" s="21"/>
+      <c r="G16" s="21"/>
+    </row>
+    <row r="17" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C17" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="D17" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="E16" s="4" t="s">
+      <c r="E17" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="F16" s="4" t="s">
+      <c r="F17" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="G16" s="4" t="s">
+      <c r="G17" s="4" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="17" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C17" s="3" t="s">
+    <row r="18" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C18" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="D18" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="E17" s="4" t="s">
+      <c r="E18" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="F17" s="4" t="s">
+      <c r="F18" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="G17" s="4" t="s">
+      <c r="G18" s="4" t="s">
         <v>99</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="C2:G2"/>
-    <mergeCell ref="C15:G15"/>
+    <mergeCell ref="C16:G16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3371,13 +3402,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C2" s="11" t="s">
         <v>89</v>
       </c>
@@ -3385,10 +3416,10 @@
         <v>90</v>
       </c>
       <c r="I2" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C3" s="10" t="s">
         <v>91</v>
       </c>
@@ -3396,14 +3427,14 @@
         <v>90</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B5" s="17" t="s">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B5" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="18"/>
-      <c r="D5" s="18"/>
-    </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C5" s="23"/>
+      <c r="D5" s="23"/>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B6" s="2" t="s">
         <v>4</v>
       </c>
@@ -3414,7 +3445,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B7" s="3" t="s">
         <v>25</v>
       </c>
@@ -3425,7 +3456,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B8" s="3" t="s">
         <v>26</v>
       </c>
@@ -3436,7 +3467,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B9" s="3" t="s">
         <v>27</v>
       </c>
@@ -3447,7 +3478,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B10" s="3" t="s">
         <v>59</v>
       </c>
@@ -3458,7 +3489,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B11" s="3" t="s">
         <v>43</v>
       </c>
@@ -3469,7 +3500,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B12" s="3" t="s">
         <v>44</v>
       </c>
@@ -3480,7 +3511,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B13" s="3" t="s">
         <v>45</v>
       </c>
@@ -3491,7 +3522,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B14" s="3" t="s">
         <v>46</v>
       </c>
@@ -3502,7 +3533,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B15" s="3" t="s">
         <v>47</v>
       </c>
@@ -3513,7 +3544,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B16" s="3" t="s">
         <v>48</v>
       </c>
@@ -3524,7 +3555,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B17" s="3" t="s">
         <v>49</v>
       </c>
@@ -3535,7 +3566,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B18" s="3" t="s">
         <v>50</v>
       </c>
@@ -3546,7 +3577,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B19" s="3" t="s">
         <v>51</v>
       </c>
@@ -3557,7 +3588,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B20" s="3" t="s">
         <v>52</v>
       </c>
@@ -3568,7 +3599,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B21" s="3" t="s">
         <v>53</v>
       </c>
@@ -3579,7 +3610,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B22" s="3" t="s">
         <v>54</v>
       </c>
@@ -3590,7 +3621,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B23" s="3" t="s">
         <v>55</v>
       </c>
@@ -3611,164 +3642,174 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3568D4F2-4AA2-4BD6-8281-861ED6398179}">
-  <dimension ref="C2:E17"/>
+  <dimension ref="C2:E18"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="22.85546875" customWidth="1"/>
+    <col min="3" max="3" width="22.88671875" customWidth="1"/>
     <col min="4" max="4" width="28" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="45" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="3:5" x14ac:dyDescent="0.3">
       <c r="D2" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="3" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="D3" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="4" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="D4" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="E2" s="12" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="3" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="D3" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="6" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C6" s="17" t="s">
+    </row>
+    <row r="7" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C7" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="D6" s="18"/>
-      <c r="E6" s="18"/>
-    </row>
-    <row r="7" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C7" s="9" t="s">
+      <c r="D7" s="23"/>
+      <c r="E7" s="23"/>
+    </row>
+    <row r="8" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C8" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="9" t="s">
+      <c r="D8" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="E8" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C8" s="3" t="s">
+    <row r="9" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C9" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D9" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="E9" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C9" s="3" t="s">
+    <row r="10" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C10" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D10" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="E10" s="4" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="10" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C10" s="3" t="s">
+    <row r="11" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C11" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D11" s="4" t="s">
         <v>77</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C11" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>79</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C12" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C13" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="E13" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C14" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="E14" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C15" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E15" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C16" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E16" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C17" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E17" s="4" t="s">
         <v>15</v>
       </c>
     </row>
+    <row r="18" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C18" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="C7:E7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3780,19 +3821,19 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="51.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="46.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="51.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="46.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B3" s="21"/>
-      <c r="C3" s="21"/>
-      <c r="G3" s="20"/>
-    </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="G11" s="19"/>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B3" s="16"/>
+      <c r="C3" s="16"/>
+      <c r="G3" s="15"/>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="G11" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Removed mqtt parameter from shadow update
</commit_message>
<xml_diff>
--- a/docs/ApplianceData.xlsx
+++ b/docs/ApplianceData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicholas.Weber.DRINKWORKS\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\espDevelopment\drinkworks-freertos\modules\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DE5D89A-22A4-4F86-A37F-951763F4A081}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63113C15-B154-4EF5-B890-21D96C4BC00E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B99E4D13-F1A0-47FA-9245-944F8FF25CEA}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{B99E4D13-F1A0-47FA-9245-944F8FF25CEA}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Overview" sheetId="3" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="97">
   <si>
     <t>Shadow Data</t>
   </si>
@@ -313,30 +313,6 @@
   </si>
   <si>
     <t>Updated Frequency:</t>
-  </si>
-  <si>
-    <t>Potential New Data</t>
-  </si>
-  <si>
-    <t>PodReady</t>
-  </si>
-  <si>
-    <t>Pod read and ready for app input</t>
-  </si>
-  <si>
-    <t>DispenseParameters</t>
-  </si>
-  <si>
-    <t>Dispense parameters ready for modification</t>
-  </si>
-  <si>
-    <t>JSON Object</t>
-  </si>
-  <si>
-    <t>On App Adjustment</t>
-  </si>
-  <si>
-    <t>Dispense Shadow</t>
   </si>
   <si>
     <t>Event Record Topic:</t>
@@ -389,7 +365,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -438,17 +414,6 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -456,7 +421,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -485,13 +450,20 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -500,16 +472,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2712,7 +2674,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{184FE990-6DFE-49C0-8AF5-25BB7F59DB88}">
   <dimension ref="C3:J29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2725,18 +2687,18 @@
   </cols>
   <sheetData>
     <row r="3" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="14"/>
-      <c r="F3" s="14" t="s">
+      <c r="D3" s="20"/>
+      <c r="F3" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="G3" s="14"/>
-      <c r="I3" s="14" t="s">
+      <c r="G3" s="20"/>
+      <c r="I3" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="J3" s="14"/>
+      <c r="J3" s="20"/>
     </row>
     <row r="4" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C4" s="2" t="s">
@@ -2959,8 +2921,8 @@
       </c>
     </row>
     <row r="15" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C15" s="23"/>
-      <c r="D15" s="23"/>
+      <c r="C15" s="18"/>
+      <c r="D15" s="18"/>
       <c r="F15" s="3" t="s">
         <v>49</v>
       </c>
@@ -2991,8 +2953,8 @@
       <c r="I17" s="8"/>
     </row>
     <row r="18" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C18" s="24"/>
-      <c r="D18" s="24"/>
+      <c r="C18" s="19"/>
+      <c r="D18" s="19"/>
       <c r="F18" s="3" t="s">
         <v>52</v>
       </c>
@@ -3002,8 +2964,8 @@
       <c r="I18" s="8"/>
     </row>
     <row r="19" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C19" s="24"/>
-      <c r="D19" s="24"/>
+      <c r="C19" s="19"/>
+      <c r="D19" s="19"/>
       <c r="F19" s="3" t="s">
         <v>53</v>
       </c>
@@ -3012,8 +2974,8 @@
       </c>
     </row>
     <row r="20" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C20" s="24"/>
-      <c r="D20" s="24"/>
+      <c r="C20" s="19"/>
+      <c r="D20" s="19"/>
       <c r="F20" s="3" t="s">
         <v>54</v>
       </c>
@@ -3037,11 +2999,11 @@
       <c r="G24" s="13"/>
     </row>
     <row r="25" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C25" s="15"/>
-      <c r="D25" s="15"/>
-      <c r="E25" s="15"/>
-      <c r="F25" s="15"/>
-      <c r="G25" s="15"/>
+      <c r="C25" s="21"/>
+      <c r="D25" s="21"/>
+      <c r="E25" s="21"/>
+      <c r="F25" s="21"/>
+      <c r="G25" s="21"/>
     </row>
     <row r="26" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C26" s="13"/>
@@ -3086,7 +3048,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC8F59E4-AA7B-4E98-A353-BDF065CC0E98}">
   <dimension ref="C2:H17"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -3100,13 +3062,13 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
     </row>
     <row r="3" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C3" s="2" t="s">
@@ -3212,11 +3174,11 @@
       </c>
     </row>
     <row r="9" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C9" s="22" t="s">
-        <v>103</v>
+      <c r="C9" s="17" t="s">
+        <v>95</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>84</v>
@@ -3314,47 +3276,25 @@
       </c>
     </row>
     <row r="15" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C15" s="16" t="s">
-        <v>92</v>
-      </c>
-      <c r="D15" s="16"/>
-      <c r="E15" s="16"/>
-      <c r="F15" s="16"/>
-      <c r="G15" s="16"/>
+      <c r="C15" s="21"/>
+      <c r="D15" s="21"/>
+      <c r="E15" s="21"/>
+      <c r="F15" s="21"/>
+      <c r="G15" s="21"/>
     </row>
     <row r="16" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C16" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="F16" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="G16" s="4" t="s">
-        <v>99</v>
-      </c>
+      <c r="C16" s="13"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="13"/>
     </row>
     <row r="17" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C17" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="F17" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="G17" s="4" t="s">
-        <v>99</v>
-      </c>
+      <c r="C17" s="13"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -3385,7 +3325,7 @@
         <v>90</v>
       </c>
       <c r="I2" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.25">
@@ -3397,11 +3337,11 @@
       </c>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="18"/>
-      <c r="D5" s="18"/>
+      <c r="C5" s="23"/>
+      <c r="D5" s="23"/>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
@@ -3624,7 +3564,7 @@
   <sheetData>
     <row r="2" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D2" s="11" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="E2" s="12" t="s">
         <v>90</v>
@@ -3635,15 +3575,15 @@
         <v>91</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
     </row>
     <row r="6" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C6" s="17" t="s">
+      <c r="C6" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="D6" s="18"/>
-      <c r="E6" s="18"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
     </row>
     <row r="7" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C7" s="9" t="s">
@@ -3787,12 +3727,12 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B3" s="21"/>
-      <c r="C3" s="21"/>
-      <c r="G3" s="20"/>
+      <c r="B3" s="16"/>
+      <c r="C3" s="16"/>
+      <c r="G3" s="15"/>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="G11" s="19"/>
+      <c r="G11" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated ApplianceData spreadsheet with correct variable names for Event Record
</commit_message>
<xml_diff>
--- a/docs/ApplianceData.xlsx
+++ b/docs/ApplianceData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ian.whitehead\GitHub\drinkworks-freertos\modules\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5739AE44-AA32-444C-B403-7A7F0500965C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7938E9D0-DA0F-4D5D-A62C-5E327DE04140}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="49663" yWindow="-1783" windowWidth="23014" windowHeight="12360" activeTab="4" xr2:uid="{B99E4D13-F1A0-47FA-9245-944F8FF25CEA}"/>
+    <workbookView xWindow="19706" yWindow="-3711" windowWidth="23014" windowHeight="12360" activeTab="3" xr2:uid="{B99E4D13-F1A0-47FA-9245-944F8FF25CEA}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Overview" sheetId="3" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="114">
   <si>
     <t>Shadow Data</t>
   </si>
@@ -343,6 +343,42 @@
   </si>
   <si>
     <t>Homebar-event-record-prod</t>
+  </si>
+  <si>
+    <t>DateTime</t>
+  </si>
+  <si>
+    <t>CycleTime</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>ISO 8601</t>
+  </si>
+  <si>
+    <t>PSI</t>
+  </si>
+  <si>
+    <t>Degrees Celcius</t>
+  </si>
+  <si>
+    <t>Seconds</t>
+  </si>
+  <si>
+    <t>e.g 2.41</t>
+  </si>
+  <si>
+    <t>Barcode #1, SKU, Beverage ID</t>
+  </si>
+  <si>
+    <t>Barcode #2, Pod ID, Formular ID</t>
+  </si>
+  <si>
+    <t>BeverageID</t>
+  </si>
+  <si>
+    <t>CatalogID</t>
   </si>
 </sst>
 </file>
@@ -438,7 +474,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -490,6 +526,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3571,51 +3610,56 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3568D4F2-4AA2-4BD6-8281-861ED6398179}">
-  <dimension ref="C2:E18"/>
+  <dimension ref="C2:F18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E25" sqref="E24:E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="22.88671875" customWidth="1"/>
     <col min="4" max="4" width="28" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="45" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.77734375" customWidth="1"/>
+    <col min="6" max="6" width="30.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="3:6" x14ac:dyDescent="0.3">
       <c r="D2" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="E2" s="26" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="3" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F2" s="26"/>
+    </row>
+    <row r="3" spans="3:6" x14ac:dyDescent="0.3">
       <c r="D3" s="11" t="s">
         <v>100</v>
       </c>
-      <c r="E3" s="12" t="s">
+      <c r="E3" s="26" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="4" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F3" s="26"/>
+    </row>
+    <row r="4" spans="3:6" x14ac:dyDescent="0.3">
       <c r="D4" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="27" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="7" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F4" s="27"/>
+    </row>
+    <row r="7" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C7" s="23" t="s">
         <v>33</v>
       </c>
       <c r="D7" s="24"/>
       <c r="E7" s="24"/>
-    </row>
-    <row r="8" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F7" s="24"/>
+    </row>
+    <row r="8" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C8" s="9" t="s">
         <v>4</v>
       </c>
@@ -3625,8 +3669,11 @@
       <c r="E8" s="2" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="9" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F8" s="9" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="9" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C9" s="3" t="s">
         <v>36</v>
       </c>
@@ -3636,10 +3683,11 @@
       <c r="E9" s="4" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="10" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F9" s="4"/>
+    </row>
+    <row r="10" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C10" s="3" t="s">
-        <v>35</v>
+        <v>102</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>75</v>
@@ -3647,8 +3695,11 @@
       <c r="E10" s="4" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="11" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F10" s="25" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="11" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C11" s="3" t="s">
         <v>14</v>
       </c>
@@ -3658,10 +3709,11 @@
       <c r="E11" s="4" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="12" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F11" s="4"/>
+    </row>
+    <row r="12" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C12" s="3" t="s">
-        <v>34</v>
+        <v>113</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>79</v>
@@ -3669,10 +3721,13 @@
       <c r="E12" s="4" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="13" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F12" s="25" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="13" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C13" s="3" t="s">
-        <v>37</v>
+        <v>103</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>78</v>
@@ -3680,8 +3735,11 @@
       <c r="E13" s="4" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="14" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F13" s="25" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="14" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C14" s="3" t="s">
         <v>38</v>
       </c>
@@ -3691,10 +3749,13 @@
       <c r="E14" s="4" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="15" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F14" s="25" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="15" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C15" s="3" t="s">
-        <v>39</v>
+        <v>112</v>
       </c>
       <c r="D15" s="4" t="s">
         <v>80</v>
@@ -3702,8 +3763,11 @@
       <c r="E15" s="4" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="16" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F15" s="25" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="16" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C16" s="3" t="s">
         <v>40</v>
       </c>
@@ -3713,8 +3777,11 @@
       <c r="E16" s="4" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F16" s="25" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="17" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C17" s="3" t="s">
         <v>41</v>
       </c>
@@ -3724,8 +3791,9 @@
       <c r="E17" s="4" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="18" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F17" s="4"/>
+    </row>
+    <row r="18" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C18" s="3" t="s">
         <v>42</v>
       </c>
@@ -3735,10 +3803,16 @@
       <c r="E18" s="4" t="s">
         <v>15</v>
       </c>
+      <c r="F18" s="25" t="s">
+        <v>107</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="C7:E7"/>
+  <mergeCells count="4">
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="C7:F7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3748,7 +3822,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FF54A45-959D-4BE7-A432-BD6A2D3FFAF4}">
   <dimension ref="B3:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>

</xml_diff>

<commit_message>
Doubled SHCI stack size due to stack overflows
</commit_message>
<xml_diff>
--- a/docs/ApplianceData.xlsx
+++ b/docs/ApplianceData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ian.whitehead\GitHub\drinkworks-freertos\modules\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\espDevelopment\drinkworks-freertos\modules\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7938E9D0-DA0F-4D5D-A62C-5E327DE04140}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49290893-F15C-46F9-81E5-E8CEF0E50E61}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19706" yWindow="-3711" windowWidth="23014" windowHeight="12360" activeTab="3" xr2:uid="{B99E4D13-F1A0-47FA-9245-944F8FF25CEA}"/>
+    <workbookView xWindow="43515" yWindow="10710" windowWidth="21600" windowHeight="11385" xr2:uid="{B99E4D13-F1A0-47FA-9245-944F8FF25CEA}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Overview" sheetId="3" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="116">
   <si>
     <t>Shadow Data</t>
   </si>
@@ -45,9 +45,6 @@
     <t>State</t>
   </si>
   <si>
-    <t>Substate</t>
-  </si>
-  <si>
     <t>MZ Firmware Version</t>
   </si>
   <si>
@@ -111,9 +108,6 @@
     <t>WaterTemp</t>
   </si>
   <si>
-    <t>HygieneStatus</t>
-  </si>
-  <si>
     <t>RunHours</t>
   </si>
   <si>
@@ -300,9 +294,6 @@
     <t>On Change</t>
   </si>
   <si>
-    <t>1m</t>
-  </si>
-  <si>
     <t>Never</t>
   </si>
   <si>
@@ -379,6 +370,21 @@
   </si>
   <si>
     <t>CatalogID</t>
+  </si>
+  <si>
+    <t>10s</t>
+  </si>
+  <si>
+    <t>SubState</t>
+  </si>
+  <si>
+    <t>LastCleanDate</t>
+  </si>
+  <si>
+    <t>Last Date Appliance was cleaned</t>
+  </si>
+  <si>
+    <t>CleanRequired</t>
   </si>
 </sst>
 </file>
@@ -474,7 +480,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -517,7 +523,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -526,9 +533,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2731,365 +2738,371 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{184FE990-6DFE-49C0-8AF5-25BB7F59DB88}">
   <dimension ref="C3:J29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15:D15"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="20.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="40.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="31.88671875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.44140625" customWidth="1"/>
+    <col min="3" max="3" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="40.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="31.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.42578125" customWidth="1"/>
     <col min="10" max="10" width="28" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C3" s="21" t="s">
+    <row r="3" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C3" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="21"/>
-      <c r="F3" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="G3" s="21"/>
-      <c r="I3" s="21" t="s">
-        <v>33</v>
-      </c>
-      <c r="J3" s="21"/>
-    </row>
-    <row r="4" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C4" s="2" t="s">
+      <c r="D3" s="23"/>
+      <c r="F3" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="G3" s="23"/>
+      <c r="I3" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="J3" s="23"/>
+    </row>
+    <row r="4" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C4" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>5</v>
-      </c>
       <c r="F4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="2" t="s">
-        <v>5</v>
-      </c>
       <c r="I4" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="J4" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="J4" s="9" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="3:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C5" s="5" t="s">
         <v>1</v>
       </c>
       <c r="D5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C6" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="D6" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F6" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="7" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C7" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F7" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="G7" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="I5" s="3" t="s">
+      <c r="I7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="8" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C8" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="J8" s="4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="9" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C9" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="J9" s="4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="10" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C10" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="I10" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="J5" s="4" t="s">
+      <c r="J10" s="4" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="6" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C6" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="D6" s="4" t="s">
+    <row r="11" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C11" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="J11" s="4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="12" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C12" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J12" s="4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="13" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C13" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="J13" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="14" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C14" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="J14" s="4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="15" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C15" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D15" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F6" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="J6" s="4" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="7" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C7" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="I7" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="J7" s="4" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="8" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C8" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="I8" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="J8" s="4" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="9" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C9" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="I9" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="J9" s="4" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="10" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C10" s="6" t="s">
+      <c r="F15" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="16" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C16" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="G10" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="I10" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="J10" s="4" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="11" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C11" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="I11" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="J11" s="4" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="12" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C12" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="G12" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="I12" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="J12" s="4" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="13" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C13" s="6" t="s">
+      <c r="D16" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D13" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="G13" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="I13" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="J13" s="4" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="14" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C14" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="F14" s="3" t="s">
+      <c r="F16" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="G14" s="4" t="s">
+      <c r="G16" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="I14" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="J14" s="4" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="15" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C15" s="19" t="s">
-        <v>96</v>
-      </c>
-      <c r="D15" s="19" t="s">
-        <v>97</v>
-      </c>
-      <c r="F15" s="3" t="s">
+      <c r="I16" s="8"/>
+    </row>
+    <row r="17" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C17" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="D17" s="19" t="s">
+        <v>94</v>
+      </c>
+      <c r="F17" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="G15" s="4" t="s">
+      <c r="G17" s="4" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="16" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C16" s="13"/>
-      <c r="D16" s="13"/>
-      <c r="F16" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="G16" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="I16" s="8"/>
-    </row>
-    <row r="17" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C17" s="13"/>
-      <c r="D17" s="13"/>
-      <c r="F17" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="G17" s="4" t="s">
-        <v>69</v>
-      </c>
       <c r="I17" s="8"/>
     </row>
-    <row r="18" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C18" s="18"/>
       <c r="D18" s="18"/>
       <c r="F18" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="I18" s="8"/>
     </row>
-    <row r="19" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C19" s="18"/>
       <c r="D19" s="18"/>
       <c r="F19" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="20" spans="3:9" x14ac:dyDescent="0.3">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="20" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C20" s="18"/>
       <c r="D20" s="18"/>
       <c r="F20" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="21" spans="3:9" x14ac:dyDescent="0.3">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="21" spans="3:9" x14ac:dyDescent="0.25">
       <c r="F21" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="24" spans="3:9" x14ac:dyDescent="0.3">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="24" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C24" s="13"/>
       <c r="D24" s="13"/>
       <c r="E24" s="13"/>
       <c r="F24" s="13"/>
       <c r="G24" s="13"/>
     </row>
-    <row r="25" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C25" s="22"/>
-      <c r="D25" s="22"/>
-      <c r="E25" s="22"/>
-      <c r="F25" s="22"/>
-      <c r="G25" s="22"/>
-    </row>
-    <row r="26" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C25" s="28"/>
+      <c r="D25" s="28"/>
+      <c r="E25" s="28"/>
+      <c r="F25" s="28"/>
+      <c r="G25" s="28"/>
+    </row>
+    <row r="26" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C26" s="13"/>
       <c r="D26" s="13"/>
       <c r="E26" s="13"/>
       <c r="F26" s="13"/>
       <c r="G26" s="13"/>
     </row>
-    <row r="27" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C27" s="13"/>
       <c r="D27" s="13"/>
       <c r="E27" s="13"/>
       <c r="F27" s="13"/>
       <c r="G27" s="13"/>
     </row>
-    <row r="28" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C28" s="13"/>
       <c r="D28" s="13"/>
       <c r="E28" s="13"/>
       <c r="F28" s="13"/>
       <c r="G28" s="13"/>
     </row>
-    <row r="29" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C29" s="13"/>
       <c r="D29" s="13"/>
       <c r="E29" s="13"/>
@@ -3097,11 +3110,10 @@
       <c r="G29" s="13"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="3">
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="F3:G3"/>
     <mergeCell ref="I3:J3"/>
-    <mergeCell ref="C25:G25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3110,250 +3122,267 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC8F59E4-AA7B-4E98-A353-BDF065CC0E98}">
-  <dimension ref="C2:H15"/>
+  <dimension ref="C2:H16"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="C3" sqref="C3:D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="19.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="40.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.109375" customWidth="1"/>
-    <col min="6" max="6" width="18.6640625" customWidth="1"/>
-    <col min="7" max="7" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="40.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.140625" customWidth="1"/>
+    <col min="6" max="6" width="18.7109375" customWidth="1"/>
+    <col min="7" max="7" width="16.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C2" s="21" t="s">
+    <row r="2" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C2" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="21"/>
-    </row>
-    <row r="3" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+    </row>
+    <row r="3" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>5</v>
-      </c>
       <c r="E3" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="H3" s="7"/>
     </row>
-    <row r="4" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C4" s="5" t="s">
         <v>1</v>
       </c>
       <c r="D4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C5" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E5" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="F5" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="F4" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="5" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C5" s="5" t="s">
+      <c r="G5" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C6" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C7" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="F7" s="22" t="s">
+        <v>84</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C8" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C9" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="E9" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C10" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C11" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C12" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C13" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C14" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D14" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E14" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F14" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="F5" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="6" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C6" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="7" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C7" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E7" s="4" t="s">
+      <c r="G14" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C15" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C16" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="D16" s="19" t="s">
+        <v>94</v>
+      </c>
+      <c r="E16" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="F16" s="20" t="s">
         <v>84</v>
       </c>
-      <c r="F7" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="8" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C8" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="9" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C9" s="17" t="s">
-        <v>94</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="10" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C10" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="G10" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="11" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C11" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="12" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C12" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="G12" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="13" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C13" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="G13" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="14" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C14" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="G14" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="15" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C15" s="19" t="s">
-        <v>96</v>
-      </c>
-      <c r="D15" s="19" t="s">
-        <v>97</v>
-      </c>
-      <c r="E15" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="F15" s="20" t="s">
-        <v>86</v>
-      </c>
-      <c r="G15" s="20" t="s">
-        <v>31</v>
+      <c r="G16" s="20" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -3370,234 +3399,234 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C2" s="11" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="D2" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="I2" t="s">
         <v>90</v>
       </c>
-      <c r="I2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C3" s="10" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B5" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="C5" s="24"/>
-      <c r="D5" s="24"/>
-    </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.3">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B5" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="25"/>
+      <c r="D5" s="25"/>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>5</v>
-      </c>
       <c r="D6" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.3">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B8" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B9" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C9" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="D7" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B8" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C8" s="4" t="s">
+      <c r="D9" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B10" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="D8" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B9" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C9" s="4" t="s">
+      <c r="C10" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="D9" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B10" s="3" t="s">
+      <c r="D10" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B11" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C11" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="D11" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B12" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C12" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="D10" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B11" s="3" t="s">
+      <c r="D12" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B13" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C13" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="D11" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B12" s="3" t="s">
+      <c r="D13" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B14" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C14" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="D12" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B13" s="3" t="s">
+      <c r="D14" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B15" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C15" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="D13" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B14" s="3" t="s">
+      <c r="D15" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B16" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C16" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="D14" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B15" s="3" t="s">
+      <c r="D16" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B17" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C17" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="D15" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B16" s="3" t="s">
+      <c r="D17" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B18" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C18" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="D16" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B17" s="3" t="s">
+      <c r="D18" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B19" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C19" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="D17" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B18" s="3" t="s">
+      <c r="D19" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B20" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C20" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="D18" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B19" s="3" t="s">
+      <c r="D20" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B21" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="C21" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="D19" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B20" s="3" t="s">
+      <c r="D21" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B22" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="C22" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="D20" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B21" s="3" t="s">
+      <c r="D22" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B23" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="C21" s="4" t="s">
+      <c r="C23" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="D21" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B22" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B23" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>73</v>
-      </c>
       <c r="D23" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -3612,199 +3641,199 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3568D4F2-4AA2-4BD6-8281-861ED6398179}">
   <dimension ref="C2:F18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E25" sqref="E24:E25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="22.88671875" customWidth="1"/>
+    <col min="3" max="3" width="22.85546875" customWidth="1"/>
     <col min="4" max="4" width="28" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30.77734375" customWidth="1"/>
-    <col min="6" max="6" width="30.33203125" customWidth="1"/>
+    <col min="5" max="5" width="30.7109375" customWidth="1"/>
+    <col min="6" max="6" width="30.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="3:6" x14ac:dyDescent="0.25">
       <c r="D2" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="E2" s="26" t="s">
+        <v>95</v>
+      </c>
+      <c r="F2" s="26"/>
+    </row>
+    <row r="3" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="D3" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="E3" s="26" t="s">
+        <v>98</v>
+      </c>
+      <c r="F3" s="26"/>
+    </row>
+    <row r="4" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="D4" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="E4" s="27" t="s">
+        <v>89</v>
+      </c>
+      <c r="F4" s="27"/>
+    </row>
+    <row r="7" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C7" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" s="25"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="25"/>
+    </row>
+    <row r="8" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C8" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="9" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C9" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" s="4"/>
+    </row>
+    <row r="10" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C10" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="E2" s="26" t="s">
-        <v>98</v>
-      </c>
-      <c r="F2" s="26"/>
-    </row>
-    <row r="3" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="D3" s="11" t="s">
+      <c r="D10" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="F10" s="22" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="11" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C11" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F11" s="4"/>
+    </row>
+    <row r="12" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C12" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F12" s="22" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="13" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C13" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="E3" s="26" t="s">
-        <v>101</v>
-      </c>
-      <c r="F3" s="26"/>
-    </row>
-    <row r="4" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="D4" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="E4" s="27" t="s">
-        <v>92</v>
-      </c>
-      <c r="F4" s="27"/>
-    </row>
-    <row r="7" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C7" s="23" t="s">
-        <v>33</v>
-      </c>
-      <c r="D7" s="24"/>
-      <c r="E7" s="24"/>
-      <c r="F7" s="24"/>
-    </row>
-    <row r="8" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C8" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D8" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F8" s="9" t="s">
+      <c r="D13" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F13" s="22" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="14" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C14" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F14" s="22" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="15" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C15" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F15" s="22" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="16" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C16" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F16" s="22" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="17" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C17" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F17" s="4"/>
+    </row>
+    <row r="18" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C18" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F18" s="22" t="s">
         <v>104</v>
-      </c>
-    </row>
-    <row r="9" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C9" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F9" s="4"/>
-    </row>
-    <row r="10" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C10" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="F10" s="25" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="11" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C11" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F11" s="4"/>
-    </row>
-    <row r="12" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C12" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F12" s="25" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="13" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C13" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F13" s="25" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="14" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C14" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F14" s="25" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="15" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C15" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F15" s="25" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="16" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C16" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F16" s="25" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="17" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C17" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F17" s="4"/>
-    </row>
-    <row r="18" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C18" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="E18" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F18" s="25" t="s">
-        <v>107</v>
       </c>
     </row>
   </sheetData>
@@ -3824,18 +3853,18 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="51.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="46.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="51.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="46.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B3" s="16"/>
       <c r="C3" s="16"/>
       <c r="G3" s="15"/>
     </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G11" s="14"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Event Record Status values to ApplianceData spreadsheet
</commit_message>
<xml_diff>
--- a/docs/ApplianceData.xlsx
+++ b/docs/ApplianceData.xlsx
@@ -1,23 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\espDevelopment\drinkworks-freertos\modules\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ian.whitehead\GitHub\drinkworks-freertos\modules\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49290893-F15C-46F9-81E5-E8CEF0E50E61}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A87D9B63-DBBA-40B5-8310-4A79F420586E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="43515" yWindow="10710" windowWidth="21600" windowHeight="11385" xr2:uid="{B99E4D13-F1A0-47FA-9245-944F8FF25CEA}"/>
+    <workbookView xWindow="22946" yWindow="-4491" windowWidth="23014" windowHeight="12360" activeTab="4" xr2:uid="{B99E4D13-F1A0-47FA-9245-944F8FF25CEA}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Overview" sheetId="3" r:id="rId1"/>
     <sheet name="Shadow Data" sheetId="1" r:id="rId2"/>
     <sheet name="Basic Ingest" sheetId="2" r:id="rId3"/>
     <sheet name="Event Records" sheetId="4" r:id="rId4"/>
-    <sheet name="Dispense Modification" sheetId="5" r:id="rId5"/>
+    <sheet name="Event Record Status" sheetId="6" r:id="rId5"/>
+    <sheet name="Dispense Modification" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="219">
   <si>
     <t>Shadow Data</t>
   </si>
@@ -385,6 +386,315 @@
   </si>
   <si>
     <t>CleanRequired</t>
+  </si>
+  <si>
+    <t>StatusText</t>
+  </si>
+  <si>
+    <t>Textual interpretation of Status</t>
+  </si>
+  <si>
+    <t>See Event Record Status tab</t>
+  </si>
+  <si>
+    <t>Dispense Completed</t>
+  </si>
+  <si>
+    <t>Error: Unknown</t>
+  </si>
+  <si>
+    <t>Error: Top-of-Tank</t>
+  </si>
+  <si>
+    <t>Error: Carbonator Fill Timeout</t>
+  </si>
+  <si>
+    <t>Error: Over Pressure</t>
+  </si>
+  <si>
+    <t>Error: Carbonation Timeout</t>
+  </si>
+  <si>
+    <t>Error: Recovery Brew</t>
+  </si>
+  <si>
+    <t>Error: Handle Lift</t>
+  </si>
+  <si>
+    <t>Error: Puncture Mechanism</t>
+  </si>
+  <si>
+    <t>Error: Carbonation Mechanism</t>
+  </si>
+  <si>
+    <t>Cleaning Cycle Completed</t>
+  </si>
+  <si>
+    <t>Rinsing Cycle Completed</t>
+  </si>
+  <si>
+    <t>CO2 Cylinder Attached</t>
+  </si>
+  <si>
+    <t>Firmware Update Passed</t>
+  </si>
+  <si>
+    <t>Firmware Update Failed</t>
+  </si>
+  <si>
+    <t>Drain Cycle Completed</t>
+  </si>
+  <si>
+    <t>Freeze Event Update</t>
+  </si>
+  <si>
+    <t>Critical Error: OverTemp</t>
+  </si>
+  <si>
+    <t>Critical Error: PuncMechFail</t>
+  </si>
+  <si>
+    <t>Critical Error: TrickleFillTmout</t>
+  </si>
+  <si>
+    <t>Critical Error: ClnRinCWTFillTmout</t>
+  </si>
+  <si>
+    <t>Critical Error: ExtendedOPError</t>
+  </si>
+  <si>
+    <t>Critical Error: BadMemClear</t>
+  </si>
+  <si>
+    <t>BLE: ModuleReset</t>
+  </si>
+  <si>
+    <t>BLE: IdleStatus</t>
+  </si>
+  <si>
+    <t>BLE: StandbyStatus</t>
+  </si>
+  <si>
+    <t>BLE: ConnectedStatus</t>
+  </si>
+  <si>
+    <t>BLE: HealthTimeout</t>
+  </si>
+  <si>
+    <t>BLE: ErrorState</t>
+  </si>
+  <si>
+    <t>BLE: MultiConnectStat</t>
+  </si>
+  <si>
+    <t>BLE: MaxCriticalTimeout</t>
+  </si>
+  <si>
+    <t>Unknown Status</t>
+  </si>
+  <si>
+    <t>0x00</t>
+  </si>
+  <si>
+    <t>eNoError</t>
+  </si>
+  <si>
+    <t>0x01</t>
+  </si>
+  <si>
+    <t>eUnknown_Error</t>
+  </si>
+  <si>
+    <t>0x02</t>
+  </si>
+  <si>
+    <t>eTop_of_Tank_Error</t>
+  </si>
+  <si>
+    <t>0x03</t>
+  </si>
+  <si>
+    <t>eCarbonator_Fill_Timeout_Error</t>
+  </si>
+  <si>
+    <t>0x04</t>
+  </si>
+  <si>
+    <t>eOver_Pressure_Error</t>
+  </si>
+  <si>
+    <t>0x05</t>
+  </si>
+  <si>
+    <t>eCarbonation_Timeout_Error</t>
+  </si>
+  <si>
+    <t>0x06</t>
+  </si>
+  <si>
+    <t>eError_Recovery_Brew</t>
+  </si>
+  <si>
+    <t>0x07</t>
+  </si>
+  <si>
+    <t>eHandle_Lift_Error</t>
+  </si>
+  <si>
+    <t>0x08</t>
+  </si>
+  <si>
+    <t>ePuncture_Mechanism_Error</t>
+  </si>
+  <si>
+    <t>0x09</t>
+  </si>
+  <si>
+    <t>eCarbonation_Mechanism_Error</t>
+  </si>
+  <si>
+    <t>0x80</t>
+  </si>
+  <si>
+    <t>eCleaning_Cycle_Completed</t>
+  </si>
+  <si>
+    <t>0x81</t>
+  </si>
+  <si>
+    <t>eRinsing_Cycle_Completed</t>
+  </si>
+  <si>
+    <t>0x82</t>
+  </si>
+  <si>
+    <t>eCO2_Module_Attached</t>
+  </si>
+  <si>
+    <t>0x83</t>
+  </si>
+  <si>
+    <t>eFirmware_Update_Passed</t>
+  </si>
+  <si>
+    <t>0x84</t>
+  </si>
+  <si>
+    <t>eFirmware_Update_Failed</t>
+  </si>
+  <si>
+    <t>0x85</t>
+  </si>
+  <si>
+    <t>eDrain_Cycle_Complete</t>
+  </si>
+  <si>
+    <t>0x86</t>
+  </si>
+  <si>
+    <t>eFreezeEventUpdate</t>
+  </si>
+  <si>
+    <t>0x87</t>
+  </si>
+  <si>
+    <t>eCritical_Error_OverTemp</t>
+  </si>
+  <si>
+    <t>0x88</t>
+  </si>
+  <si>
+    <t>eCritical_Error_PuncMechFail</t>
+  </si>
+  <si>
+    <t>0x89</t>
+  </si>
+  <si>
+    <t>eCritical_Error_TrickleFillTmout</t>
+  </si>
+  <si>
+    <t>0x8A</t>
+  </si>
+  <si>
+    <t>eCritical_Error_ClnRinCWTFillTmout</t>
+  </si>
+  <si>
+    <t>0x8B</t>
+  </si>
+  <si>
+    <t>eCritical_Error_ExtendedOPError</t>
+  </si>
+  <si>
+    <t>0x8C</t>
+  </si>
+  <si>
+    <t>eCritical_Error_BadMemClear</t>
+  </si>
+  <si>
+    <t>0xE0</t>
+  </si>
+  <si>
+    <t>eBLE_ModuleReset</t>
+  </si>
+  <si>
+    <t>0xE1</t>
+  </si>
+  <si>
+    <t>eBLE_IdleStatus</t>
+  </si>
+  <si>
+    <t>0xE2</t>
+  </si>
+  <si>
+    <t>eBLE_StandbyStatus</t>
+  </si>
+  <si>
+    <t>0xE3</t>
+  </si>
+  <si>
+    <t>eBLE_ConnectedStatus</t>
+  </si>
+  <si>
+    <t>0xE4</t>
+  </si>
+  <si>
+    <t>eBLE_HealthTimeout</t>
+  </si>
+  <si>
+    <t>0xE5</t>
+  </si>
+  <si>
+    <t>eBLE_ErrorState</t>
+  </si>
+  <si>
+    <t>0xE6</t>
+  </si>
+  <si>
+    <t>eBLE_MultiConnectStat</t>
+  </si>
+  <si>
+    <t>0xE7</t>
+  </si>
+  <si>
+    <t>eBLE_MaxCriticalTimeout</t>
+  </si>
+  <si>
+    <t>0xFF</t>
+  </si>
+  <si>
+    <t>eUnknownStatus</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>Enumerated Value</t>
+  </si>
+  <si>
+    <t>Event Record Status</t>
+  </si>
+  <si>
+    <t>Textual Interpretation (string)</t>
   </si>
 </sst>
 </file>
@@ -480,7 +790,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -527,6 +837,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -535,7 +849,16 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2738,33 +3061,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{184FE990-6DFE-49C0-8AF5-25BB7F59DB88}">
   <dimension ref="C3:J29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="40.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="31.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.42578125" customWidth="1"/>
+    <col min="3" max="3" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="40.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="31.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.44140625" customWidth="1"/>
     <col min="10" max="10" width="28" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C3" s="23" t="s">
+    <row r="3" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C3" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="23"/>
-      <c r="F3" s="23" t="s">
+      <c r="D3" s="25"/>
+      <c r="F3" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="G3" s="23"/>
-      <c r="I3" s="23" t="s">
+      <c r="G3" s="25"/>
+      <c r="I3" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="J3" s="23"/>
-    </row>
-    <row r="4" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="J3" s="25"/>
+    </row>
+    <row r="4" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C4" s="21" t="s">
         <v>3</v>
       </c>
@@ -2784,7 +3107,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C5" s="5" t="s">
         <v>1</v>
       </c>
@@ -2804,7 +3127,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="6" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C6" s="5" t="s">
         <v>112</v>
       </c>
@@ -2824,7 +3147,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="7" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C7" s="5" t="s">
         <v>22</v>
       </c>
@@ -2844,7 +3167,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="8" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C8" s="5" t="s">
         <v>113</v>
       </c>
@@ -2864,7 +3187,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="9" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C9" s="5" t="s">
         <v>115</v>
       </c>
@@ -2884,7 +3207,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="10" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C10" s="5" t="s">
         <v>15</v>
       </c>
@@ -2904,7 +3227,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="11" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C11" s="17" t="s">
         <v>91</v>
       </c>
@@ -2924,7 +3247,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="12" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C12" s="6" t="s">
         <v>16</v>
       </c>
@@ -2944,7 +3267,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="13" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C13" s="6" t="s">
         <v>18</v>
       </c>
@@ -2964,7 +3287,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="14" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C14" s="6" t="s">
         <v>19</v>
       </c>
@@ -2984,7 +3307,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="15" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C15" s="6" t="s">
         <v>20</v>
       </c>
@@ -2998,7 +3321,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="16" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C16" s="6" t="s">
         <v>17</v>
       </c>
@@ -3013,7 +3336,7 @@
       </c>
       <c r="I16" s="8"/>
     </row>
-    <row r="17" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C17" s="19" t="s">
         <v>93</v>
       </c>
@@ -3028,7 +3351,7 @@
       </c>
       <c r="I17" s="8"/>
     </row>
-    <row r="18" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C18" s="18"/>
       <c r="D18" s="18"/>
       <c r="F18" s="3" t="s">
@@ -3039,7 +3362,7 @@
       </c>
       <c r="I18" s="8"/>
     </row>
-    <row r="19" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C19" s="18"/>
       <c r="D19" s="18"/>
       <c r="F19" s="3" t="s">
@@ -3049,7 +3372,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="20" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C20" s="18"/>
       <c r="D20" s="18"/>
       <c r="F20" s="3" t="s">
@@ -3059,7 +3382,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="21" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:9" x14ac:dyDescent="0.3">
       <c r="F21" s="3" t="s">
         <v>53</v>
       </c>
@@ -3067,42 +3390,42 @@
         <v>71</v>
       </c>
     </row>
-    <row r="24" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C24" s="13"/>
       <c r="D24" s="13"/>
       <c r="E24" s="13"/>
       <c r="F24" s="13"/>
       <c r="G24" s="13"/>
     </row>
-    <row r="25" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C25" s="28"/>
-      <c r="D25" s="28"/>
-      <c r="E25" s="28"/>
-      <c r="F25" s="28"/>
-      <c r="G25" s="28"/>
-    </row>
-    <row r="26" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C25" s="24"/>
+      <c r="D25" s="24"/>
+      <c r="E25" s="24"/>
+      <c r="F25" s="24"/>
+      <c r="G25" s="24"/>
+    </row>
+    <row r="26" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C26" s="13"/>
       <c r="D26" s="13"/>
       <c r="E26" s="13"/>
       <c r="F26" s="13"/>
       <c r="G26" s="13"/>
     </row>
-    <row r="27" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C27" s="13"/>
       <c r="D27" s="13"/>
       <c r="E27" s="13"/>
       <c r="F27" s="13"/>
       <c r="G27" s="13"/>
     </row>
-    <row r="28" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C28" s="13"/>
       <c r="D28" s="13"/>
       <c r="E28" s="13"/>
       <c r="F28" s="13"/>
       <c r="G28" s="13"/>
     </row>
-    <row r="29" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C29" s="13"/>
       <c r="D29" s="13"/>
       <c r="E29" s="13"/>
@@ -3128,25 +3451,25 @@
       <selection activeCell="C3" sqref="C3:D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="40.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.140625" customWidth="1"/>
-    <col min="6" max="6" width="18.7109375" customWidth="1"/>
-    <col min="7" max="7" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="40.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.109375" customWidth="1"/>
+    <col min="6" max="6" width="18.6640625" customWidth="1"/>
+    <col min="7" max="7" width="16.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C2" s="23" t="s">
+    <row r="2" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C2" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-    </row>
-    <row r="3" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+    </row>
+    <row r="3" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C3" s="2" t="s">
         <v>3</v>
       </c>
@@ -3164,7 +3487,7 @@
       </c>
       <c r="H3" s="7"/>
     </row>
-    <row r="4" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C4" s="5" t="s">
         <v>1</v>
       </c>
@@ -3181,7 +3504,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C5" s="5" t="s">
         <v>112</v>
       </c>
@@ -3198,7 +3521,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C6" s="5" t="s">
         <v>22</v>
       </c>
@@ -3215,7 +3538,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C7" s="5" t="s">
         <v>113</v>
       </c>
@@ -3232,7 +3555,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C8" s="5" t="s">
         <v>115</v>
       </c>
@@ -3249,7 +3572,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C9" s="5" t="s">
         <v>15</v>
       </c>
@@ -3266,7 +3589,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C10" s="17" t="s">
         <v>91</v>
       </c>
@@ -3283,7 +3606,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C11" s="6" t="s">
         <v>16</v>
       </c>
@@ -3300,7 +3623,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C12" s="6" t="s">
         <v>18</v>
       </c>
@@ -3317,7 +3640,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C13" s="6" t="s">
         <v>19</v>
       </c>
@@ -3334,7 +3657,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C14" s="6" t="s">
         <v>20</v>
       </c>
@@ -3351,7 +3674,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C15" s="6" t="s">
         <v>17</v>
       </c>
@@ -3368,7 +3691,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C16" s="19" t="s">
         <v>93</v>
       </c>
@@ -3399,13 +3722,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C2" s="11" t="s">
         <v>86</v>
       </c>
@@ -3416,7 +3739,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C3" s="10" t="s">
         <v>88</v>
       </c>
@@ -3424,14 +3747,14 @@
         <v>87</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B5" s="24" t="s">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B5" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="C5" s="25"/>
-      <c r="D5" s="25"/>
-    </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C5" s="27"/>
+      <c r="D5" s="27"/>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B6" s="2" t="s">
         <v>3</v>
       </c>
@@ -3442,7 +3765,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B7" s="3" t="s">
         <v>23</v>
       </c>
@@ -3453,7 +3776,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B8" s="3" t="s">
         <v>24</v>
       </c>
@@ -3464,7 +3787,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B9" s="3" t="s">
         <v>25</v>
       </c>
@@ -3475,7 +3798,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B10" s="3" t="s">
         <v>57</v>
       </c>
@@ -3486,7 +3809,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B11" s="3" t="s">
         <v>41</v>
       </c>
@@ -3497,7 +3820,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B12" s="3" t="s">
         <v>42</v>
       </c>
@@ -3508,7 +3831,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B13" s="3" t="s">
         <v>43</v>
       </c>
@@ -3519,7 +3842,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B14" s="3" t="s">
         <v>44</v>
       </c>
@@ -3530,7 +3853,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B15" s="3" t="s">
         <v>45</v>
       </c>
@@ -3541,7 +3864,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B16" s="3" t="s">
         <v>46</v>
       </c>
@@ -3552,7 +3875,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B17" s="3" t="s">
         <v>47</v>
       </c>
@@ -3563,7 +3886,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B18" s="3" t="s">
         <v>48</v>
       </c>
@@ -3574,7 +3897,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B19" s="3" t="s">
         <v>49</v>
       </c>
@@ -3585,7 +3908,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B20" s="3" t="s">
         <v>50</v>
       </c>
@@ -3596,7 +3919,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B21" s="3" t="s">
         <v>51</v>
       </c>
@@ -3607,7 +3930,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B22" s="3" t="s">
         <v>52</v>
       </c>
@@ -3618,7 +3941,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B23" s="3" t="s">
         <v>53</v>
       </c>
@@ -3639,56 +3962,56 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3568D4F2-4AA2-4BD6-8281-861ED6398179}">
-  <dimension ref="C2:F18"/>
+  <dimension ref="C2:F19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E25" sqref="E24:E25"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="22.85546875" customWidth="1"/>
+    <col min="3" max="3" width="22.88671875" customWidth="1"/>
     <col min="4" max="4" width="28" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30.7109375" customWidth="1"/>
-    <col min="6" max="6" width="30.28515625" customWidth="1"/>
+    <col min="5" max="5" width="30.6640625" customWidth="1"/>
+    <col min="6" max="6" width="30.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="3:6" x14ac:dyDescent="0.3">
       <c r="D2" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="E2" s="26" t="s">
+      <c r="E2" s="28" t="s">
         <v>95</v>
       </c>
-      <c r="F2" s="26"/>
-    </row>
-    <row r="3" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="F2" s="28"/>
+    </row>
+    <row r="3" spans="3:6" x14ac:dyDescent="0.3">
       <c r="D3" s="11" t="s">
         <v>97</v>
       </c>
-      <c r="E3" s="26" t="s">
+      <c r="E3" s="28" t="s">
         <v>98</v>
       </c>
-      <c r="F3" s="26"/>
-    </row>
-    <row r="4" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="F3" s="28"/>
+    </row>
+    <row r="4" spans="3:6" x14ac:dyDescent="0.3">
       <c r="D4" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="E4" s="27" t="s">
+      <c r="E4" s="29" t="s">
         <v>89</v>
       </c>
-      <c r="F4" s="27"/>
-    </row>
-    <row r="7" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C7" s="24" t="s">
+      <c r="F4" s="29"/>
+    </row>
+    <row r="7" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C7" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="D7" s="25"/>
-      <c r="E7" s="25"/>
-      <c r="F7" s="25"/>
-    </row>
-    <row r="8" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="D7" s="27"/>
+      <c r="E7" s="27"/>
+      <c r="F7" s="27"/>
+    </row>
+    <row r="8" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C8" s="9" t="s">
         <v>3</v>
       </c>
@@ -3702,7 +4025,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="9" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C9" s="3" t="s">
         <v>34</v>
       </c>
@@ -3714,7 +4037,7 @@
       </c>
       <c r="F9" s="4"/>
     </row>
-    <row r="10" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C10" s="3" t="s">
         <v>99</v>
       </c>
@@ -3728,7 +4051,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="11" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C11" s="3" t="s">
         <v>13</v>
       </c>
@@ -3740,99 +4063,113 @@
       </c>
       <c r="F11" s="4"/>
     </row>
-    <row r="12" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C12" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="13" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C13" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="D13" s="4" t="s">
         <v>77</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F12" s="22" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="13" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C13" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>76</v>
       </c>
       <c r="E13" s="4" t="s">
         <v>14</v>
       </c>
       <c r="F13" s="22" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="14" spans="3:6" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="14" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C14" s="3" t="s">
-        <v>36</v>
+        <v>100</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E14" s="4" t="s">
         <v>14</v>
       </c>
       <c r="F14" s="22" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="15" spans="3:6" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="15" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C15" s="3" t="s">
-        <v>109</v>
+        <v>36</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="E15" s="4" t="s">
         <v>14</v>
       </c>
       <c r="F15" s="22" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="16" spans="3:6" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="16" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C16" s="3" t="s">
-        <v>38</v>
+        <v>109</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E16" s="4" t="s">
         <v>14</v>
       </c>
       <c r="F16" s="22" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="17" spans="3:6" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="17" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C17" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E17" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="F17" s="4"/>
-    </row>
-    <row r="18" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="F17" s="22" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="18" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C18" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E18" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="F18" s="22" t="s">
+      <c r="F18" s="4"/>
+    </row>
+    <row r="19" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C19" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F19" s="22" t="s">
         <v>104</v>
       </c>
     </row>
@@ -3848,23 +4185,417 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5BD56E4-EBF7-4AF2-A6CB-E8AE0371B992}">
+  <dimension ref="B1:D34"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="8.88671875" style="30"/>
+    <col min="3" max="3" width="36.5546875" customWidth="1"/>
+    <col min="4" max="4" width="38.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B1" s="31" t="s">
+        <v>217</v>
+      </c>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+    </row>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B2" s="23" t="s">
+        <v>215</v>
+      </c>
+      <c r="C2" s="32" t="s">
+        <v>216</v>
+      </c>
+      <c r="D2" s="32" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B3" s="33" t="s">
+        <v>151</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B4" s="33" t="s">
+        <v>153</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B5" s="33" t="s">
+        <v>155</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B6" s="33" t="s">
+        <v>157</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B7" s="33" t="s">
+        <v>159</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B8" s="33" t="s">
+        <v>161</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B9" s="33" t="s">
+        <v>163</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B10" s="33" t="s">
+        <v>165</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B11" s="33" t="s">
+        <v>167</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B12" s="33" t="s">
+        <v>169</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B13" s="33" t="s">
+        <v>171</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B14" s="33" t="s">
+        <v>173</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B15" s="33" t="s">
+        <v>175</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B16" s="33" t="s">
+        <v>177</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B17" s="33" t="s">
+        <v>179</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B18" s="33" t="s">
+        <v>181</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B19" s="33" t="s">
+        <v>183</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B20" s="33" t="s">
+        <v>185</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B21" s="33" t="s">
+        <v>187</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B22" s="33" t="s">
+        <v>189</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B23" s="33" t="s">
+        <v>191</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B24" s="33" t="s">
+        <v>193</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B25" s="33" t="s">
+        <v>195</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B26" s="33" t="s">
+        <v>197</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B27" s="33" t="s">
+        <v>199</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B28" s="33" t="s">
+        <v>201</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B29" s="33" t="s">
+        <v>203</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="30" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B30" s="33" t="s">
+        <v>205</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B31" s="33" t="s">
+        <v>207</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="32" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B32" s="33" t="s">
+        <v>209</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B33" s="33" t="s">
+        <v>211</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>212</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B34" s="33" t="s">
+        <v>213</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>150</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:D1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FF54A45-959D-4BE7-A432-BD6A2D3FFAF4}">
   <dimension ref="B3:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="51.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="46.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="51.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="46.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B3" s="16"/>
       <c r="C3" s="16"/>
       <c r="G3" s="15"/>
     </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:7" x14ac:dyDescent="0.3">
       <c r="G11" s="14"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated shadow documentation to include MinToChilled
</commit_message>
<xml_diff>
--- a/docs/ApplianceData.xlsx
+++ b/docs/ApplianceData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ian.whitehead\GitHub\drinkworks-freertos\modules\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\espDevelopment\drinkworks-freertos\modules\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A87D9B63-DBBA-40B5-8310-4A79F420586E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30BC5DE0-AEB6-4AE8-9BA5-52860364901F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22946" yWindow="-4491" windowWidth="23014" windowHeight="12360" activeTab="4" xr2:uid="{B99E4D13-F1A0-47FA-9245-944F8FF25CEA}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B99E4D13-F1A0-47FA-9245-944F8FF25CEA}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Overview" sheetId="3" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="222">
   <si>
     <t>Shadow Data</t>
   </si>
@@ -695,6 +695,15 @@
   </si>
   <si>
     <t>Textual Interpretation (string)</t>
+  </si>
+  <si>
+    <t>MinToChilled</t>
+  </si>
+  <si>
+    <t>Min until appliance is cold enough for carb bevs</t>
+  </si>
+  <si>
+    <t>On Chnge</t>
   </si>
 </sst>
 </file>
@@ -838,6 +847,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -849,14 +865,7 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -3061,33 +3070,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{184FE990-6DFE-49C0-8AF5-25BB7F59DB88}">
   <dimension ref="C3:J29"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="20.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="40.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="31.88671875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.44140625" customWidth="1"/>
+    <col min="3" max="3" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="43.28515625" customWidth="1"/>
+    <col min="6" max="6" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="31.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.42578125" customWidth="1"/>
     <col min="10" max="10" width="28" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C3" s="25" t="s">
+    <row r="3" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C3" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="25"/>
-      <c r="F3" s="25" t="s">
+      <c r="D3" s="28"/>
+      <c r="F3" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="G3" s="25"/>
-      <c r="I3" s="25" t="s">
+      <c r="G3" s="28"/>
+      <c r="I3" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="J3" s="25"/>
-    </row>
-    <row r="4" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="J3" s="28"/>
+    </row>
+    <row r="4" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C4" s="21" t="s">
         <v>3</v>
       </c>
@@ -3107,7 +3116,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C5" s="5" t="s">
         <v>1</v>
       </c>
@@ -3127,7 +3136,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="6" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C6" s="5" t="s">
         <v>112</v>
       </c>
@@ -3147,7 +3156,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="7" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C7" s="5" t="s">
         <v>22</v>
       </c>
@@ -3167,7 +3176,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="8" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C8" s="5" t="s">
         <v>113</v>
       </c>
@@ -3187,7 +3196,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="9" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C9" s="5" t="s">
         <v>115</v>
       </c>
@@ -3207,7 +3216,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="10" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C10" s="5" t="s">
         <v>15</v>
       </c>
@@ -3227,7 +3236,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="11" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C11" s="17" t="s">
         <v>91</v>
       </c>
@@ -3247,7 +3256,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="12" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C12" s="6" t="s">
         <v>16</v>
       </c>
@@ -3267,7 +3276,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="13" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C13" s="6" t="s">
         <v>18</v>
       </c>
@@ -3287,7 +3296,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="14" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C14" s="6" t="s">
         <v>19</v>
       </c>
@@ -3307,7 +3316,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="15" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C15" s="6" t="s">
         <v>20</v>
       </c>
@@ -3321,7 +3330,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="16" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C16" s="6" t="s">
         <v>17</v>
       </c>
@@ -3336,7 +3345,7 @@
       </c>
       <c r="I16" s="8"/>
     </row>
-    <row r="17" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C17" s="19" t="s">
         <v>93</v>
       </c>
@@ -3351,9 +3360,13 @@
       </c>
       <c r="I17" s="8"/>
     </row>
-    <row r="18" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
+    <row r="18" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C18" s="17" t="s">
+        <v>219</v>
+      </c>
+      <c r="D18" s="19" t="s">
+        <v>220</v>
+      </c>
       <c r="F18" s="3" t="s">
         <v>50</v>
       </c>
@@ -3362,7 +3375,7 @@
       </c>
       <c r="I18" s="8"/>
     </row>
-    <row r="19" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C19" s="18"/>
       <c r="D19" s="18"/>
       <c r="F19" s="3" t="s">
@@ -3372,7 +3385,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="20" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C20" s="18"/>
       <c r="D20" s="18"/>
       <c r="F20" s="3" t="s">
@@ -3382,7 +3395,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="21" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="3:9" x14ac:dyDescent="0.25">
       <c r="F21" s="3" t="s">
         <v>53</v>
       </c>
@@ -3390,42 +3403,42 @@
         <v>71</v>
       </c>
     </row>
-    <row r="24" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C24" s="13"/>
       <c r="D24" s="13"/>
       <c r="E24" s="13"/>
       <c r="F24" s="13"/>
       <c r="G24" s="13"/>
     </row>
-    <row r="25" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C25" s="24"/>
       <c r="D25" s="24"/>
       <c r="E25" s="24"/>
       <c r="F25" s="24"/>
       <c r="G25" s="24"/>
     </row>
-    <row r="26" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C26" s="13"/>
       <c r="D26" s="13"/>
       <c r="E26" s="13"/>
       <c r="F26" s="13"/>
       <c r="G26" s="13"/>
     </row>
-    <row r="27" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C27" s="13"/>
       <c r="D27" s="13"/>
       <c r="E27" s="13"/>
       <c r="F27" s="13"/>
       <c r="G27" s="13"/>
     </row>
-    <row r="28" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C28" s="13"/>
       <c r="D28" s="13"/>
       <c r="E28" s="13"/>
       <c r="F28" s="13"/>
       <c r="G28" s="13"/>
     </row>
-    <row r="29" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C29" s="13"/>
       <c r="D29" s="13"/>
       <c r="E29" s="13"/>
@@ -3445,31 +3458,31 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC8F59E4-AA7B-4E98-A353-BDF065CC0E98}">
-  <dimension ref="C2:H16"/>
+  <dimension ref="C2:H17"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:D16"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="19.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="40.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.109375" customWidth="1"/>
-    <col min="6" max="6" width="18.6640625" customWidth="1"/>
-    <col min="7" max="7" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="40.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.140625" customWidth="1"/>
+    <col min="6" max="6" width="18.7109375" customWidth="1"/>
+    <col min="7" max="7" width="16.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C2" s="25" t="s">
+    <row r="2" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C2" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-    </row>
-    <row r="3" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+    </row>
+    <row r="3" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C3" s="2" t="s">
         <v>3</v>
       </c>
@@ -3487,7 +3500,7 @@
       </c>
       <c r="H3" s="7"/>
     </row>
-    <row r="4" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C4" s="5" t="s">
         <v>1</v>
       </c>
@@ -3504,7 +3517,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C5" s="5" t="s">
         <v>112</v>
       </c>
@@ -3521,7 +3534,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C6" s="5" t="s">
         <v>22</v>
       </c>
@@ -3538,7 +3551,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C7" s="5" t="s">
         <v>113</v>
       </c>
@@ -3555,7 +3568,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C8" s="5" t="s">
         <v>115</v>
       </c>
@@ -3572,7 +3585,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C9" s="5" t="s">
         <v>15</v>
       </c>
@@ -3589,7 +3602,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C10" s="17" t="s">
         <v>91</v>
       </c>
@@ -3606,7 +3619,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C11" s="6" t="s">
         <v>16</v>
       </c>
@@ -3623,7 +3636,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C12" s="6" t="s">
         <v>18</v>
       </c>
@@ -3640,7 +3653,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C13" s="6" t="s">
         <v>19</v>
       </c>
@@ -3657,7 +3670,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C14" s="6" t="s">
         <v>20</v>
       </c>
@@ -3674,7 +3687,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C15" s="6" t="s">
         <v>17</v>
       </c>
@@ -3691,7 +3704,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C16" s="19" t="s">
         <v>93</v>
       </c>
@@ -3705,6 +3718,23 @@
         <v>84</v>
       </c>
       <c r="G16" s="20" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C17" s="17" t="s">
+        <v>219</v>
+      </c>
+      <c r="D17" s="19" t="s">
+        <v>220</v>
+      </c>
+      <c r="E17" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="F17" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="G17" s="22" t="s">
         <v>29</v>
       </c>
     </row>
@@ -3722,13 +3752,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C2" s="11" t="s">
         <v>86</v>
       </c>
@@ -3739,7 +3769,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C3" s="10" t="s">
         <v>88</v>
       </c>
@@ -3747,14 +3777,14 @@
         <v>87</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B5" s="26" t="s">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B5" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="C5" s="27"/>
-      <c r="D5" s="27"/>
-    </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="C5" s="30"/>
+      <c r="D5" s="30"/>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>3</v>
       </c>
@@ -3765,7 +3795,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
         <v>23</v>
       </c>
@@ -3776,7 +3806,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
         <v>24</v>
       </c>
@@ -3787,7 +3817,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
         <v>25</v>
       </c>
@@ -3798,7 +3828,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B10" s="3" t="s">
         <v>57</v>
       </c>
@@ -3809,7 +3839,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B11" s="3" t="s">
         <v>41</v>
       </c>
@@ -3820,7 +3850,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B12" s="3" t="s">
         <v>42</v>
       </c>
@@ -3831,7 +3861,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B13" s="3" t="s">
         <v>43</v>
       </c>
@@ -3842,7 +3872,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B14" s="3" t="s">
         <v>44</v>
       </c>
@@ -3853,7 +3883,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B15" s="3" t="s">
         <v>45</v>
       </c>
@@ -3864,7 +3894,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B16" s="3" t="s">
         <v>46</v>
       </c>
@@ -3875,7 +3905,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" s="3" t="s">
         <v>47</v>
       </c>
@@ -3886,7 +3916,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" s="3" t="s">
         <v>48</v>
       </c>
@@ -3897,7 +3927,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B19" s="3" t="s">
         <v>49</v>
       </c>
@@ -3908,7 +3938,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" s="3" t="s">
         <v>50</v>
       </c>
@@ -3919,7 +3949,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21" s="3" t="s">
         <v>51</v>
       </c>
@@ -3930,7 +3960,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B22" s="3" t="s">
         <v>52</v>
       </c>
@@ -3941,7 +3971,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B23" s="3" t="s">
         <v>53</v>
       </c>
@@ -3968,50 +3998,50 @@
       <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="22.88671875" customWidth="1"/>
+    <col min="3" max="3" width="22.85546875" customWidth="1"/>
     <col min="4" max="4" width="28" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30.6640625" customWidth="1"/>
-    <col min="6" max="6" width="30.33203125" customWidth="1"/>
+    <col min="5" max="5" width="30.7109375" customWidth="1"/>
+    <col min="6" max="6" width="30.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="3:6" x14ac:dyDescent="0.25">
       <c r="D2" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="E2" s="28" t="s">
+      <c r="E2" s="31" t="s">
         <v>95</v>
       </c>
-      <c r="F2" s="28"/>
-    </row>
-    <row r="3" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="F2" s="31"/>
+    </row>
+    <row r="3" spans="3:6" x14ac:dyDescent="0.25">
       <c r="D3" s="11" t="s">
         <v>97</v>
       </c>
-      <c r="E3" s="28" t="s">
+      <c r="E3" s="31" t="s">
         <v>98</v>
       </c>
-      <c r="F3" s="28"/>
-    </row>
-    <row r="4" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="F3" s="31"/>
+    </row>
+    <row r="4" spans="3:6" x14ac:dyDescent="0.25">
       <c r="D4" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="E4" s="29" t="s">
+      <c r="E4" s="32" t="s">
         <v>89</v>
       </c>
-      <c r="F4" s="29"/>
-    </row>
-    <row r="7" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C7" s="26" t="s">
+      <c r="F4" s="32"/>
+    </row>
+    <row r="7" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C7" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="D7" s="27"/>
-      <c r="E7" s="27"/>
-      <c r="F7" s="27"/>
-    </row>
-    <row r="8" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="D7" s="30"/>
+      <c r="E7" s="30"/>
+      <c r="F7" s="30"/>
+    </row>
+    <row r="8" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C8" s="9" t="s">
         <v>3</v>
       </c>
@@ -4025,7 +4055,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="9" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C9" s="3" t="s">
         <v>34</v>
       </c>
@@ -4037,7 +4067,7 @@
       </c>
       <c r="F9" s="4"/>
     </row>
-    <row r="10" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C10" s="3" t="s">
         <v>99</v>
       </c>
@@ -4051,7 +4081,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="11" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C11" s="3" t="s">
         <v>13</v>
       </c>
@@ -4063,7 +4093,7 @@
       </c>
       <c r="F11" s="4"/>
     </row>
-    <row r="12" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C12" s="3" t="s">
         <v>116</v>
       </c>
@@ -4077,7 +4107,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="13" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C13" s="3" t="s">
         <v>110</v>
       </c>
@@ -4091,7 +4121,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="14" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C14" s="3" t="s">
         <v>100</v>
       </c>
@@ -4105,7 +4135,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="15" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C15" s="3" t="s">
         <v>36</v>
       </c>
@@ -4119,7 +4149,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="16" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C16" s="3" t="s">
         <v>109</v>
       </c>
@@ -4133,7 +4163,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="17" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C17" s="3" t="s">
         <v>38</v>
       </c>
@@ -4147,7 +4177,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="18" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C18" s="3" t="s">
         <v>39</v>
       </c>
@@ -4159,7 +4189,7 @@
       </c>
       <c r="F18" s="4"/>
     </row>
-    <row r="19" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C19" s="3" t="s">
         <v>40</v>
       </c>
@@ -4188,37 +4218,37 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5BD56E4-EBF7-4AF2-A6CB-E8AE0371B992}">
   <dimension ref="B1:D34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="8.88671875" style="30"/>
-    <col min="3" max="3" width="36.5546875" customWidth="1"/>
-    <col min="4" max="4" width="38.44140625" customWidth="1"/>
+    <col min="2" max="2" width="8.85546875" style="25"/>
+    <col min="3" max="3" width="36.5703125" customWidth="1"/>
+    <col min="4" max="4" width="38.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B1" s="31" t="s">
+    <row r="1" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B1" s="33" t="s">
         <v>217</v>
       </c>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-    </row>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+    </row>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B2" s="23" t="s">
         <v>215</v>
       </c>
-      <c r="C2" s="32" t="s">
+      <c r="C2" s="26" t="s">
         <v>216</v>
       </c>
-      <c r="D2" s="32" t="s">
+      <c r="D2" s="26" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B3" s="33" t="s">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B3" s="27" t="s">
         <v>151</v>
       </c>
       <c r="C3" s="4" t="s">
@@ -4228,8 +4258,8 @@
         <v>119</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B4" s="33" t="s">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B4" s="27" t="s">
         <v>153</v>
       </c>
       <c r="C4" s="4" t="s">
@@ -4239,8 +4269,8 @@
         <v>120</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B5" s="33" t="s">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B5" s="27" t="s">
         <v>155</v>
       </c>
       <c r="C5" s="4" t="s">
@@ -4250,8 +4280,8 @@
         <v>121</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B6" s="33" t="s">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B6" s="27" t="s">
         <v>157</v>
       </c>
       <c r="C6" s="4" t="s">
@@ -4261,8 +4291,8 @@
         <v>122</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B7" s="33" t="s">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B7" s="27" t="s">
         <v>159</v>
       </c>
       <c r="C7" s="4" t="s">
@@ -4272,8 +4302,8 @@
         <v>123</v>
       </c>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B8" s="33" t="s">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B8" s="27" t="s">
         <v>161</v>
       </c>
       <c r="C8" s="4" t="s">
@@ -4283,8 +4313,8 @@
         <v>124</v>
       </c>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B9" s="33" t="s">
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B9" s="27" t="s">
         <v>163</v>
       </c>
       <c r="C9" s="4" t="s">
@@ -4294,8 +4324,8 @@
         <v>125</v>
       </c>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B10" s="33" t="s">
+    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B10" s="27" t="s">
         <v>165</v>
       </c>
       <c r="C10" s="4" t="s">
@@ -4305,8 +4335,8 @@
         <v>126</v>
       </c>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B11" s="33" t="s">
+    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B11" s="27" t="s">
         <v>167</v>
       </c>
       <c r="C11" s="4" t="s">
@@ -4316,8 +4346,8 @@
         <v>127</v>
       </c>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B12" s="33" t="s">
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B12" s="27" t="s">
         <v>169</v>
       </c>
       <c r="C12" s="4" t="s">
@@ -4327,8 +4357,8 @@
         <v>128</v>
       </c>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B13" s="33" t="s">
+    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B13" s="27" t="s">
         <v>171</v>
       </c>
       <c r="C13" s="4" t="s">
@@ -4338,8 +4368,8 @@
         <v>129</v>
       </c>
     </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B14" s="33" t="s">
+    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B14" s="27" t="s">
         <v>173</v>
       </c>
       <c r="C14" s="4" t="s">
@@ -4349,8 +4379,8 @@
         <v>130</v>
       </c>
     </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B15" s="33" t="s">
+    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B15" s="27" t="s">
         <v>175</v>
       </c>
       <c r="C15" s="4" t="s">
@@ -4360,8 +4390,8 @@
         <v>131</v>
       </c>
     </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B16" s="33" t="s">
+    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B16" s="27" t="s">
         <v>177</v>
       </c>
       <c r="C16" s="4" t="s">
@@ -4371,8 +4401,8 @@
         <v>132</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B17" s="33" t="s">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B17" s="27" t="s">
         <v>179</v>
       </c>
       <c r="C17" s="4" t="s">
@@ -4382,8 +4412,8 @@
         <v>133</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B18" s="33" t="s">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B18" s="27" t="s">
         <v>181</v>
       </c>
       <c r="C18" s="4" t="s">
@@ -4393,8 +4423,8 @@
         <v>134</v>
       </c>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B19" s="33" t="s">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B19" s="27" t="s">
         <v>183</v>
       </c>
       <c r="C19" s="4" t="s">
@@ -4404,8 +4434,8 @@
         <v>135</v>
       </c>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B20" s="33" t="s">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B20" s="27" t="s">
         <v>185</v>
       </c>
       <c r="C20" s="4" t="s">
@@ -4415,8 +4445,8 @@
         <v>136</v>
       </c>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B21" s="33" t="s">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B21" s="27" t="s">
         <v>187</v>
       </c>
       <c r="C21" s="4" t="s">
@@ -4426,8 +4456,8 @@
         <v>137</v>
       </c>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B22" s="33" t="s">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B22" s="27" t="s">
         <v>189</v>
       </c>
       <c r="C22" s="4" t="s">
@@ -4437,8 +4467,8 @@
         <v>138</v>
       </c>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B23" s="33" t="s">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B23" s="27" t="s">
         <v>191</v>
       </c>
       <c r="C23" s="4" t="s">
@@ -4448,8 +4478,8 @@
         <v>139</v>
       </c>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B24" s="33" t="s">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B24" s="27" t="s">
         <v>193</v>
       </c>
       <c r="C24" s="4" t="s">
@@ -4459,8 +4489,8 @@
         <v>140</v>
       </c>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B25" s="33" t="s">
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B25" s="27" t="s">
         <v>195</v>
       </c>
       <c r="C25" s="4" t="s">
@@ -4470,8 +4500,8 @@
         <v>141</v>
       </c>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B26" s="33" t="s">
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B26" s="27" t="s">
         <v>197</v>
       </c>
       <c r="C26" s="4" t="s">
@@ -4481,8 +4511,8 @@
         <v>142</v>
       </c>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B27" s="33" t="s">
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B27" s="27" t="s">
         <v>199</v>
       </c>
       <c r="C27" s="4" t="s">
@@ -4492,8 +4522,8 @@
         <v>143</v>
       </c>
     </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B28" s="33" t="s">
+    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B28" s="27" t="s">
         <v>201</v>
       </c>
       <c r="C28" s="4" t="s">
@@ -4503,8 +4533,8 @@
         <v>144</v>
       </c>
     </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B29" s="33" t="s">
+    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B29" s="27" t="s">
         <v>203</v>
       </c>
       <c r="C29" s="4" t="s">
@@ -4514,8 +4544,8 @@
         <v>145</v>
       </c>
     </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B30" s="33" t="s">
+    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B30" s="27" t="s">
         <v>205</v>
       </c>
       <c r="C30" s="4" t="s">
@@ -4525,8 +4555,8 @@
         <v>146</v>
       </c>
     </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B31" s="33" t="s">
+    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B31" s="27" t="s">
         <v>207</v>
       </c>
       <c r="C31" s="4" t="s">
@@ -4536,8 +4566,8 @@
         <v>147</v>
       </c>
     </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B32" s="33" t="s">
+    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B32" s="27" t="s">
         <v>209</v>
       </c>
       <c r="C32" s="4" t="s">
@@ -4547,8 +4577,8 @@
         <v>148</v>
       </c>
     </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B33" s="33" t="s">
+    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B33" s="27" t="s">
         <v>211</v>
       </c>
       <c r="C33" s="4" t="s">
@@ -4558,8 +4588,8 @@
         <v>149</v>
       </c>
     </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B34" s="33" t="s">
+    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B34" s="27" t="s">
         <v>213</v>
       </c>
       <c r="C34" s="4" t="s">
@@ -4584,18 +4614,18 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="51.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="46.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="51.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="46.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B3" s="16"/>
       <c r="C3" s="16"/>
       <c r="G3" s="15"/>
     </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G11" s="14"/>
     </row>
   </sheetData>

</xml_diff>